<commit_message>
adjusting events + icons
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I852780\Desktop\football team\footballteam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfc90\Desktop\Footballteam\footballteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{562B3186-94E8-47B9-9283-B1817F28F4A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D01304-F151-4094-96F3-F604B1E3FBB8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{8647F8B8-294B-49BC-B5F8-C94F475E1A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t>You need to pass in the difficulty test 3 times</t>
-  </si>
-  <si>
-    <t>Shoot</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Hat-trick</t>
   </si>
@@ -39,21 +33,12 @@
     <t>Free Kick</t>
   </si>
   <si>
-    <t>2,2,3</t>
-  </si>
-  <si>
-    <t>Defence Pass Shoot</t>
-  </si>
-  <si>
     <t>Counterattack</t>
   </si>
   <si>
     <t>2 VP</t>
   </si>
   <si>
-    <t>Defence</t>
-  </si>
-  <si>
     <t>Defend against the Counterattack</t>
   </si>
   <si>
@@ -66,20 +51,59 @@
     <t>Reward</t>
   </si>
   <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Events</t>
+  </si>
+  <si>
+    <t>3 VP</t>
+  </si>
+  <si>
+    <t>4 VP</t>
+  </si>
+  <si>
+    <t>5 VP</t>
+  </si>
+  <si>
+    <t>More rewards go here blablablabla</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Difficulty1</t>
+  </si>
+  <si>
+    <t>Difficulty2</t>
+  </si>
+  <si>
+    <t>Difficulty3</t>
+  </si>
+  <si>
+    <t>Difficulty4</t>
+  </si>
+  <si>
+    <t>shooting.svg</t>
+  </si>
+  <si>
+    <t>defence.svg</t>
+  </si>
+  <si>
+    <t>assisting.svg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -88,6 +112,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,14 +145,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -438,117 +471,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BEBC7F1-EE45-4B6D-B9A1-C2B94529B8F7}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="K6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed deck number of cards
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I852780\Desktop\football team\footballteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A15BEE01-F7B4-4414-80E6-BBADBABFDA99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{93162508-7C0C-4BE3-89C8-74E0394FDAF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{8647F8B8-294B-49BC-B5F8-C94F475E1A1D}"/>
   </bookViews>
@@ -159,13 +159,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -486,7 +483,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -504,28 +501,28 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -546,20 +543,20 @@
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>3</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="1"/>
@@ -752,7 +749,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="M10" s="6"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>

</xml_diff>